<commit_message>
update on test report
</commit_message>
<xml_diff>
--- a/Workbook2.xlsx
+++ b/Workbook2.xlsx
@@ -596,9 +596,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>1-if the candidate opens list of companies the keyboard shows up and this is confused us.</t>
-  </si>
-  <si>
     <t>the icon of upload cv is not mached its functionality</t>
   </si>
   <si>
@@ -660,22 +657,18 @@
   </si>
   <si>
     <t xml:space="preserve">add to favorite button exist in organizational information that is already in  favorite category organization </t>
+  </si>
+  <si>
+    <t>if the candidate opens list of companies the keyboard shows up and this is confused us.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1061,33 +1054,33 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1099,9 +1092,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1112,43 +1102,120 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1160,32 +1227,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1195,71 +1244,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1587,8 +1571,8 @@
   </sheetPr>
   <dimension ref="C1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="42" zoomScaleNormal="71" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E3"/>
+    <sheetView tabSelected="1" topLeftCell="K19" zoomScale="42" zoomScaleNormal="71" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1613,28 +1597,28 @@
   <sheetData>
     <row r="1" spans="3:5" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="3:5" ht="37" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="49"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="51"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
     </row>
     <row r="3" spans="3:5" ht="38" x14ac:dyDescent="0.35">
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
     </row>
     <row r="4" spans="3:5" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
     </row>
     <row r="5" spans="3:5" ht="38.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="44"/>
     </row>
     <row r="6" spans="3:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C6" s="4" t="s">
@@ -1692,118 +1676,118 @@
       </c>
     </row>
     <row r="11" spans="3:5" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="C11" s="60"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
     </row>
     <row r="12" spans="3:5" ht="20.5" x14ac:dyDescent="0.35">
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="47"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
     </row>
     <row r="13" spans="3:5" ht="20.5" x14ac:dyDescent="0.35">
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="48"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
     </row>
     <row r="14" spans="3:5" ht="20.5" x14ac:dyDescent="0.35">
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="48"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" spans="3:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="3:5" ht="20" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="45"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="3:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="33"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
     </row>
     <row r="21" spans="3:5" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="22" spans="3:5" ht="31" x14ac:dyDescent="0.7">
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="38"/>
-      <c r="E23" s="39"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="65"/>
     </row>
     <row r="24" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="39"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="65"/>
     </row>
     <row r="25" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="39"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="65"/>
     </row>
     <row r="26" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="39"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="65"/>
     </row>
     <row r="27" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="38"/>
-      <c r="E27" s="39"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="65"/>
     </row>
     <row r="28" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="39"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="65"/>
     </row>
     <row r="29" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
     </row>
     <row r="30" spans="3:5" ht="21" x14ac:dyDescent="0.5">
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="24"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="50"/>
     </row>
     <row r="31" spans="3:5" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="53"/>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C34" s="1" t="s">
@@ -1859,34 +1843,34 @@
       <c r="D35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E35" s="20">
+      <c r="E35" s="18">
         <v>43076</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G35" s="63">
+      <c r="G35" s="20">
         <v>43081</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I35" s="16" t="s">
+      <c r="I35" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="J35" s="16" t="s">
+      <c r="J35" s="15" t="s">
         <v>42</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L35" s="16" t="s">
+      <c r="L35" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="M35" s="16" t="s">
+      <c r="M35" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N35" s="16" t="s">
+      <c r="N35" s="15" t="s">
         <v>44</v>
       </c>
       <c r="O35" s="10" t="s">
@@ -1895,8 +1879,8 @@
       <c r="P35" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Q35" s="64" t="s">
-        <v>99</v>
+      <c r="Q35" s="16" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="3:17" s="1" customFormat="1" ht="186" customHeight="1" x14ac:dyDescent="0.35">
@@ -1906,44 +1890,44 @@
       <c r="D36" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="20">
+      <c r="E36" s="18">
         <v>43076</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="G36" s="65">
+      <c r="G36" s="21">
         <v>43081</v>
       </c>
-      <c r="H36" s="16" t="s">
+      <c r="H36" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="16" t="s">
+      <c r="I36" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J36" s="16" t="s">
+      <c r="J36" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L36" s="16" t="s">
+      <c r="L36" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="M36" s="16" t="s">
+      <c r="M36" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="N36" s="16" t="s">
+      <c r="N36" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="O36" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="P36" s="17" t="s">
+      <c r="O36" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="Q36" s="18" t="s">
+      <c r="P36" s="16" t="s">
         <v>100</v>
+      </c>
+      <c r="Q36" s="16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="3:17" s="1" customFormat="1" ht="108.5" x14ac:dyDescent="0.35">
@@ -1953,44 +1937,44 @@
       <c r="D37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E37" s="20">
+      <c r="E37" s="18">
         <v>43076</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F37" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="G37" s="65">
+      <c r="G37" s="21">
         <v>43081</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I37" s="16" t="s">
+      <c r="I37" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J37" s="16" t="s">
+      <c r="J37" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="M37" s="16" t="s">
+      <c r="M37" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N37" s="16" t="s">
+      <c r="N37" s="15" t="s">
         <v>48</v>
       </c>
       <c r="O37" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P37" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Q37" s="13" t="s">
-        <v>106</v>
+      <c r="Q37" s="16" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="3:17" s="1" customFormat="1" ht="137" customHeight="1" x14ac:dyDescent="0.35">
@@ -2000,44 +1984,44 @@
       <c r="D38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="18">
         <v>43076</v>
       </c>
       <c r="F38" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="G38" s="63">
+      <c r="G38" s="20">
         <v>43081</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="I38" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="J38" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L38" s="16" t="s">
+      <c r="L38" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="M38" s="16" t="s">
+      <c r="M38" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N38" s="16" t="s">
+      <c r="N38" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="O38" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="P38" s="17" t="s">
+      <c r="O38" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="P38" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q38" s="18" t="s">
-        <v>110</v>
+      <c r="Q38" s="16" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="3:17" s="1" customFormat="1" ht="145" customHeight="1" x14ac:dyDescent="0.35">
@@ -2047,43 +2031,43 @@
       <c r="D39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E39" s="20">
+      <c r="E39" s="18">
         <v>43076</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G39" s="66">
+        <v>102</v>
+      </c>
+      <c r="G39" s="22">
         <v>43081</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="16" t="s">
+      <c r="I39" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="J39" s="16" t="s">
+      <c r="J39" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L39" s="16" t="s">
+      <c r="L39" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="M39" s="16" t="s">
+      <c r="M39" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N39" s="16" t="s">
+      <c r="N39" s="15" t="s">
         <v>56</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="P39" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="Q39" s="13"/>
+      <c r="Q39" s="16"/>
     </row>
     <row r="40" spans="3:17" ht="155" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
@@ -2092,43 +2076,43 @@
       <c r="D40" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="20">
+      <c r="E40" s="18">
         <v>43076</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G40" s="67">
+        <v>102</v>
+      </c>
+      <c r="G40" s="23">
         <v>43081</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="16" t="s">
+      <c r="I40" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J40" s="16" t="s">
+      <c r="J40" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K40" s="16" t="s">
+      <c r="K40" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L40" s="16" t="s">
+      <c r="L40" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="M40" s="21" t="s">
+      <c r="M40" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="N40" s="16" t="s">
+      <c r="N40" s="15" t="s">
         <v>72</v>
       </c>
       <c r="O40" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="P40" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="P40" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q40" s="15"/>
+      <c r="Q40" s="16"/>
     </row>
     <row r="41" spans="3:17" ht="233" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
@@ -2137,44 +2121,44 @@
       <c r="D41" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="18">
         <v>43076</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" s="66">
+        <v>102</v>
+      </c>
+      <c r="G41" s="22">
         <v>43081</v>
       </c>
-      <c r="H41" s="16" t="s">
+      <c r="H41" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="16" t="s">
+      <c r="I41" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K41" s="16" t="s">
+      <c r="K41" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="M41" s="16" t="s">
+      <c r="M41" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N41" s="16" t="s">
+      <c r="N41" s="15" t="s">
         <v>85</v>
       </c>
       <c r="O41" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="P41" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q41" s="16" t="s">
         <v>119</v>
-      </c>
-      <c r="P41" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q41" s="14" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="42" spans="3:17" ht="170.5" x14ac:dyDescent="0.35">
@@ -2184,44 +2168,44 @@
       <c r="D42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="20">
+      <c r="E42" s="18">
         <v>43076</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="G42" s="66">
+        <v>102</v>
+      </c>
+      <c r="G42" s="22">
         <v>43081</v>
       </c>
-      <c r="H42" s="16" t="s">
+      <c r="H42" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="I42" s="16" t="s">
+      <c r="I42" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J42" s="15" t="s">
         <v>38</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L42" s="16" t="s">
+      <c r="L42" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="M42" s="16" t="s">
+      <c r="M42" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N42" s="16" t="s">
+      <c r="N42" s="15" t="s">
         <v>58</v>
       </c>
       <c r="O42" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="P42" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="P42" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q42" s="15" t="s">
-        <v>118</v>
+      <c r="Q42" s="16" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="3:17" ht="200" customHeight="1" x14ac:dyDescent="0.35">
@@ -2231,43 +2215,43 @@
       <c r="D43" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E43" s="20">
+      <c r="E43" s="18">
         <v>43076</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="67">
+        <v>103</v>
+      </c>
+      <c r="G43" s="23">
         <v>43081</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K43" s="16" t="s">
+      <c r="K43" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L43" s="16" t="s">
+      <c r="L43" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="M43" s="16" t="s">
+      <c r="M43" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N43" s="16" t="s">
+      <c r="N43" s="15" t="s">
         <v>62</v>
       </c>
       <c r="O43" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="P43" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="Q43" s="14"/>
+      <c r="P43" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q43" s="16"/>
     </row>
     <row r="44" spans="3:17" ht="217" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
@@ -2276,44 +2260,44 @@
       <c r="D44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E44" s="20">
+      <c r="E44" s="18">
         <v>43076</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G44" s="66">
+        <v>103</v>
+      </c>
+      <c r="G44" s="22">
         <v>43081</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I44" s="16" t="s">
+      <c r="I44" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="J44" s="16" t="s">
+      <c r="J44" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K44" s="16" t="s">
+      <c r="K44" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="L44" s="16" t="s">
+      <c r="L44" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="M44" s="16" t="s">
+      <c r="M44" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="N44" s="16" t="s">
+      <c r="N44" s="15" t="s">
         <v>65</v>
       </c>
       <c r="O44" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="P44" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="P44" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q44" s="15" t="s">
-        <v>118</v>
+      <c r="Q44" s="16" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="3:17" ht="248" customHeight="1" x14ac:dyDescent="0.35">
@@ -2323,81 +2307,81 @@
       <c r="D45" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="18">
         <v>43076</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G45" s="67">
+        <v>103</v>
+      </c>
+      <c r="G45" s="23">
         <v>43081</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I45" s="16" t="s">
+      <c r="I45" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J45" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="K45" s="16" t="s">
+      <c r="K45" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="L45" s="16" t="s">
+      <c r="L45" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="M45" s="16" t="s">
+      <c r="M45" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="N45" s="16" t="s">
+      <c r="N45" s="15" t="s">
         <v>69</v>
       </c>
       <c r="O45" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="P45" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="P45" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="Q45" s="14"/>
+      <c r="Q45" s="16"/>
     </row>
     <row r="46" spans="3:17" ht="161" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>12</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="20"/>
+      <c r="E46" s="18"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
-      <c r="M46" s="16"/>
-      <c r="N46" s="16"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
+      <c r="K46" s="15"/>
+      <c r="L46" s="15"/>
+      <c r="M46" s="15"/>
+      <c r="N46" s="15"/>
       <c r="O46" s="9"/>
       <c r="P46" s="9"/>
-      <c r="Q46" s="15"/>
+      <c r="Q46" s="14"/>
     </row>
     <row r="47" spans="3:17" ht="141" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>13</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" s="20"/>
+      <c r="E47" s="18"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="16"/>
-      <c r="J47" s="16"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="16"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="16"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="15"/>
+      <c r="L47" s="15"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="15"/>
       <c r="O47" s="9"/>
       <c r="P47" s="11"/>
-      <c r="Q47" s="14"/>
+      <c r="Q47" s="13"/>
     </row>
     <row r="48" spans="3:17" ht="139" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
@@ -2408,15 +2392,15 @@
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15"/>
+      <c r="M48" s="15"/>
+      <c r="N48" s="15"/>
       <c r="O48" s="9"/>
       <c r="P48" s="9"/>
-      <c r="Q48" s="15"/>
+      <c r="Q48" s="14"/>
     </row>
     <row r="49" spans="3:17" ht="136" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
@@ -2427,15 +2411,15 @@
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="16"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="16"/>
-      <c r="M49" s="19"/>
-      <c r="N49" s="16"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="15"/>
       <c r="O49" s="9"/>
       <c r="P49" s="11"/>
-      <c r="Q49" s="14"/>
+      <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="3:17" ht="135" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
@@ -2446,15 +2430,15 @@
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="16"/>
-      <c r="J50" s="16"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="16"/>
-      <c r="M50" s="16"/>
-      <c r="N50" s="16"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
+      <c r="K50" s="15"/>
+      <c r="L50" s="15"/>
+      <c r="M50" s="15"/>
+      <c r="N50" s="15"/>
       <c r="O50" s="9"/>
       <c r="P50" s="9"/>
-      <c r="Q50" s="15"/>
+      <c r="Q50" s="14"/>
     </row>
     <row r="51" spans="3:17" ht="125" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
@@ -2465,15 +2449,15 @@
       <c r="F51" s="11"/>
       <c r="G51" s="11"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
       <c r="N51" s="1"/>
       <c r="O51" s="9"/>
       <c r="P51" s="11"/>
-      <c r="Q51" s="14"/>
+      <c r="Q51" s="13"/>
     </row>
     <row r="52" spans="3:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
@@ -2484,15 +2468,15 @@
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="16"/>
-      <c r="M52" s="16"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+      <c r="M52" s="15"/>
       <c r="N52" s="1"/>
       <c r="O52" s="9"/>
       <c r="P52" s="9"/>
-      <c r="Q52" s="15"/>
+      <c r="Q52" s="14"/>
     </row>
     <row r="53" spans="3:17" ht="110" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
@@ -2503,15 +2487,15 @@
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="16"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="16"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
       <c r="M53" s="1"/>
-      <c r="N53" s="16"/>
+      <c r="N53" s="15"/>
       <c r="O53" s="9"/>
       <c r="P53" s="11"/>
-      <c r="Q53" s="14"/>
+      <c r="Q53" s="13"/>
     </row>
     <row r="54" spans="3:17" ht="109" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
@@ -2522,28 +2506,18 @@
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="16"/>
-      <c r="J54" s="16"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="16"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
+      <c r="K54" s="15"/>
+      <c r="L54" s="15"/>
       <c r="M54" s="1"/>
-      <c r="N54" s="16"/>
+      <c r="N54" s="15"/>
       <c r="O54" s="9"/>
       <c r="P54" s="9"/>
-      <c r="Q54" s="15"/>
+      <c r="Q54" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C11:E11"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C29:E29"/>
@@ -2555,8 +2529,18 @@
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C27:E27"/>
     <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C11:E11"/>
   </mergeCells>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" fitToWidth="2" fitToHeight="2" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>